<commit_message>
Remove more HM functionality
</commit_message>
<xml_diff>
--- a/CodeErrorTracker.xlsx
+++ b/CodeErrorTracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Masters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0E3CAE8-BF8D-431F-8E65-46EEBEDC4A7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3825E672-10D1-4C4D-A9E7-FC165BA5B1AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{706D98CE-F3E1-459F-8932-AE27958A7F32}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="173">
   <si>
     <t>File</t>
   </si>
@@ -577,6 +577,9 @@
   </si>
   <si>
     <t>Look into other papers 2015 2018 and other for MEC theory</t>
+  </si>
+  <si>
+    <t>Try to visualize mat A and B to make sure it looks right</t>
   </si>
 </sst>
 </file>
@@ -4367,10 +4370,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{746B74A1-E2E9-411E-A31B-49675430CC3B}">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4408,6 +4411,11 @@
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>171</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removal of more hm
</commit_message>
<xml_diff>
--- a/CodeErrorTracker.xlsx
+++ b/CodeErrorTracker.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Masters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3825E672-10D1-4C4D-A9E7-FC165BA5B1AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD7484D5-AC4A-4A7B-965E-FD150FBFAC7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{706D98CE-F3E1-459F-8932-AE27958A7F32}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="176">
   <si>
     <t>File</t>
   </si>
@@ -579,7 +579,16 @@
     <t>Look into other papers 2015 2018 and other for MEC theory</t>
   </si>
   <si>
-    <t>Try to visualize mat A and B to make sure it looks right</t>
+    <t>Changing the phase rotation and the inOut does not change the magnitude. My leading theory is that the ur, sigma, rel, MMF or other params of nodes in MEC regions are wrong</t>
+  </si>
+  <si>
+    <t>Changing the MMF scaling to always be ppSlotHeight (max) does not change magnitude or waveform</t>
+  </si>
+  <si>
+    <t>Changing reluctance does change magnitude</t>
+  </si>
+  <si>
+    <t>Is it possible that the error exists in the x direction code. I always skip that assuming its right but there may be errors</t>
   </si>
 </sst>
 </file>
@@ -4370,10 +4379,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{746B74A1-E2E9-411E-A31B-49675430CC3B}">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:A14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4416,6 +4425,21 @@
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>172</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>175</v>
       </c>
     </row>
   </sheetData>

</xml_diff>